<commit_message>
hyperparameter tuning for meta subclasses
</commit_message>
<xml_diff>
--- a/4_classification&evaluation/output/meta_subclasses/evaluation_metrics.xlsx
+++ b/4_classification&evaluation/output/meta_subclasses/evaluation_metrics.xlsx
@@ -562,16 +562,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5952380952380951</v>
+        <v>0.6228571428571429</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5597246642246642</v>
+        <v>0.6028299319727891</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5952380952380951</v>
+        <v>0.6228571428571429</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5302161814793394</v>
+        <v>0.5631802054154995</v>
       </c>
       <c r="F2" t="n">
         <v>0.7552380952380952</v>
@@ -586,52 +586,52 @@
         <v>0.7321976911976911</v>
       </c>
       <c r="J2" t="n">
-        <v>0.7542857142857142</v>
+        <v>0.7685714285714285</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7597142857142858</v>
+        <v>0.8038095238095238</v>
       </c>
       <c r="L2" t="n">
-        <v>0.7542857142857142</v>
+        <v>0.7685714285714285</v>
       </c>
       <c r="M2" t="n">
-        <v>0.7280434961863532</v>
+        <v>0.7549641311069882</v>
       </c>
       <c r="N2" t="n">
-        <v>0.5933333333333334</v>
+        <v>0.8114285714285714</v>
       </c>
       <c r="O2" t="n">
-        <v>0.4133679653679653</v>
+        <v>0.8068253968253968</v>
       </c>
       <c r="P2" t="n">
-        <v>0.5933333333333334</v>
+        <v>0.8114285714285714</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.469703081232493</v>
+        <v>0.7898923298923299</v>
       </c>
       <c r="R2" t="n">
-        <v>0.5133333333333334</v>
+        <v>0.580952380952381</v>
       </c>
       <c r="S2" t="n">
-        <v>0.3504945054945056</v>
+        <v>0.5471395271395272</v>
       </c>
       <c r="T2" t="n">
-        <v>0.5133333333333334</v>
+        <v>0.580952380952381</v>
       </c>
       <c r="U2" t="n">
-        <v>0.3802256621947024</v>
+        <v>0.4939516192441888</v>
       </c>
       <c r="V2" t="n">
-        <v>0.4733333333333333</v>
+        <v>0.580952380952381</v>
       </c>
       <c r="W2" t="n">
-        <v>0.3024945054945055</v>
+        <v>0.5635031635031635</v>
       </c>
       <c r="X2" t="n">
-        <v>0.4733333333333333</v>
+        <v>0.580952380952381</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.3326066145756548</v>
+        <v>0.4948143643422281</v>
       </c>
     </row>
     <row r="3">
@@ -878,28 +878,28 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.7161904761904763</v>
+        <v>0.7028571428571428</v>
       </c>
       <c r="C6" t="n">
-        <v>0.720937950937951</v>
+        <v>0.7156046176046177</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7161904761904763</v>
+        <v>0.7028571428571428</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6765703614779246</v>
+        <v>0.6605703614779245</v>
       </c>
       <c r="F6" t="n">
-        <v>0.798095238095238</v>
+        <v>0.8114285714285714</v>
       </c>
       <c r="G6" t="n">
-        <v>0.7711746031746032</v>
+        <v>0.7911746031746032</v>
       </c>
       <c r="H6" t="n">
-        <v>0.798095238095238</v>
+        <v>0.8114285714285714</v>
       </c>
       <c r="I6" t="n">
-        <v>0.7581414141414141</v>
+        <v>0.7760461760461761</v>
       </c>
       <c r="J6" t="n">
         <v>0.7714285714285715</v>
@@ -914,40 +914,40 @@
         <v>0.7318556998556998</v>
       </c>
       <c r="N6" t="n">
-        <v>0.7438095238095237</v>
+        <v>0.7438095238095238</v>
       </c>
       <c r="O6" t="n">
-        <v>0.7325649350649351</v>
+        <v>0.726374458874459</v>
       </c>
       <c r="P6" t="n">
-        <v>0.7438095238095237</v>
+        <v>0.7438095238095238</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.6994791352438412</v>
+        <v>0.6975255332902393</v>
       </c>
       <c r="R6" t="n">
         <v>0.7171428571428571</v>
       </c>
       <c r="S6" t="n">
-        <v>0.6930411255411255</v>
+        <v>0.7025649350649351</v>
       </c>
       <c r="T6" t="n">
         <v>0.7171428571428571</v>
       </c>
       <c r="U6" t="n">
-        <v>0.6678747396394454</v>
+        <v>0.6627807225454284</v>
       </c>
       <c r="V6" t="n">
-        <v>0.7295238095238096</v>
+        <v>0.7428571428571429</v>
       </c>
       <c r="W6" t="n">
-        <v>0.711111111111111</v>
+        <v>0.7273015873015873</v>
       </c>
       <c r="X6" t="n">
-        <v>0.7295238095238096</v>
+        <v>0.7428571428571429</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.6841779173207744</v>
+        <v>0.6956553287981858</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix in context integration
</commit_message>
<xml_diff>
--- a/4_classification&evaluation/output/meta_subclasses/evaluation_metrics.xlsx
+++ b/4_classification&evaluation/output/meta_subclasses/evaluation_metrics.xlsx
@@ -890,16 +890,16 @@
         <v>0.6605703614779245</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8114285714285714</v>
+        <v>0.798095238095238</v>
       </c>
       <c r="G6" t="n">
-        <v>0.7911746031746032</v>
+        <v>0.7678412698412698</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8114285714285714</v>
+        <v>0.798095238095238</v>
       </c>
       <c r="I6" t="n">
-        <v>0.7760461760461761</v>
+        <v>0.756998556998557</v>
       </c>
       <c r="J6" t="n">
         <v>0.7714285714285715</v>
@@ -914,40 +914,40 @@
         <v>0.7318556998556998</v>
       </c>
       <c r="N6" t="n">
-        <v>0.7438095238095238</v>
+        <v>0.7704761904761905</v>
       </c>
       <c r="O6" t="n">
-        <v>0.726374458874459</v>
+        <v>0.7492316017316017</v>
       </c>
       <c r="P6" t="n">
-        <v>0.7438095238095238</v>
+        <v>0.7704761904761905</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.6975255332902393</v>
+        <v>0.7255743733390793</v>
       </c>
       <c r="R6" t="n">
-        <v>0.7171428571428571</v>
+        <v>0.7304761904761905</v>
       </c>
       <c r="S6" t="n">
-        <v>0.7025649350649351</v>
+        <v>0.7195346320346321</v>
       </c>
       <c r="T6" t="n">
-        <v>0.7171428571428571</v>
+        <v>0.7304761904761905</v>
       </c>
       <c r="U6" t="n">
-        <v>0.6627807225454284</v>
+        <v>0.6792513107807225</v>
       </c>
       <c r="V6" t="n">
-        <v>0.7428571428571429</v>
+        <v>0.7295238095238095</v>
       </c>
       <c r="W6" t="n">
-        <v>0.7273015873015873</v>
+        <v>0.7086349206349206</v>
       </c>
       <c r="X6" t="n">
-        <v>0.7428571428571429</v>
+        <v>0.7295238095238095</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.6956553287981858</v>
+        <v>0.6783219954648526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>